<commit_message>
edited calcIdealAngles2 function, changed to correct units (radians) for all angles
</commit_message>
<xml_diff>
--- a/clino_accessible_scattering_planes.xlsx
+++ b/clino_accessible_scattering_planes.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -522,32 +522,32 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>hk02</t>
+          <t>-hk0</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="C3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D3" t="n">
         <v>0</v>
       </c>
       <c r="E3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G3" t="n">
         <v>0</v>
       </c>
       <c r="H3" t="n">
-        <v>16.3655482504197</v>
+        <v>16.36557946754619</v>
       </c>
       <c r="I3" t="n">
-        <v>15.24705525689201</v>
+        <v>15.24571639765113</v>
       </c>
       <c r="J3" t="n">
         <v>1</v>
@@ -556,11 +556,11 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>-hk0</t>
+          <t>hkk</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="C4" t="n">
         <v>0</v>
@@ -575,13 +575,13 @@
         <v>1</v>
       </c>
       <c r="G4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H4" t="n">
-        <v>16.36557946754619</v>
+        <v>-20.38790312912558</v>
       </c>
       <c r="I4" t="n">
-        <v>15.24571639765113</v>
+        <v>14.75155044961241</v>
       </c>
       <c r="J4" t="n">
         <v>1</v>
@@ -590,11 +590,11 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>hkk</t>
+          <t>-hkk</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="C5" t="n">
         <v>0</v>
@@ -612,10 +612,10 @@
         <v>1</v>
       </c>
       <c r="H5" t="n">
-        <v>-20.38790312912558</v>
+        <v>-20.38798492004405</v>
       </c>
       <c r="I5" t="n">
-        <v>14.75155044961241</v>
+        <v>14.75057443453965</v>
       </c>
       <c r="J5" t="n">
         <v>1</v>
@@ -624,18 +624,18 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>-hkk</t>
+          <t>hk-h</t>
         </is>
       </c>
       <c r="B6" t="n">
+        <v>1</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0</v>
+      </c>
+      <c r="D6" t="n">
         <v>-1</v>
       </c>
-      <c r="C6" t="n">
-        <v>0</v>
-      </c>
-      <c r="D6" t="n">
-        <v>0</v>
-      </c>
       <c r="E6" t="n">
         <v>0</v>
       </c>
@@ -643,13 +643,13 @@
         <v>1</v>
       </c>
       <c r="G6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H6" t="n">
-        <v>-20.38798492004405</v>
+        <v>39.89501358610413</v>
       </c>
       <c r="I6" t="n">
-        <v>14.75057443453965</v>
+        <v>84.38029043267113</v>
       </c>
       <c r="J6" t="n">
         <v>1</v>
@@ -658,7 +658,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>hk-h</t>
+          <t>hk-k</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -668,22 +668,22 @@
         <v>0</v>
       </c>
       <c r="D7" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F7" t="n">
+        <v>1</v>
+      </c>
+      <c r="G7" t="n">
         <v>-1</v>
       </c>
-      <c r="E7" t="n">
-        <v>0</v>
-      </c>
-      <c r="F7" t="n">
-        <v>1</v>
-      </c>
-      <c r="G7" t="n">
-        <v>0</v>
-      </c>
       <c r="H7" t="n">
-        <v>39.89501358610413</v>
+        <v>53.11834447701406</v>
       </c>
       <c r="I7" t="n">
-        <v>84.38029043267113</v>
+        <v>15.03092225791461</v>
       </c>
       <c r="J7" t="n">
         <v>1</v>
@@ -692,11 +692,11 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>hk-k</t>
+          <t>-hk-k</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="C8" t="n">
         <v>0</v>
@@ -714,46 +714,12 @@
         <v>-1</v>
       </c>
       <c r="H8" t="n">
-        <v>53.11834447701406</v>
+        <v>53.11831356662042</v>
       </c>
       <c r="I8" t="n">
-        <v>15.03092225791461</v>
+        <v>15.03048069096935</v>
       </c>
       <c r="J8" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>-hk-k</t>
-        </is>
-      </c>
-      <c r="B9" t="n">
-        <v>-1</v>
-      </c>
-      <c r="C9" t="n">
-        <v>0</v>
-      </c>
-      <c r="D9" t="n">
-        <v>0</v>
-      </c>
-      <c r="E9" t="n">
-        <v>0</v>
-      </c>
-      <c r="F9" t="n">
-        <v>1</v>
-      </c>
-      <c r="G9" t="n">
-        <v>-1</v>
-      </c>
-      <c r="H9" t="n">
-        <v>53.11831356662042</v>
-      </c>
-      <c r="I9" t="n">
-        <v>15.03048069096935</v>
-      </c>
-      <c r="J9" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>